<commit_message>
add battle damage / exp gained
</commit_message>
<xml_diff>
--- a/PKMN_BackUp/PKMN_PokemonHold.xlsx
+++ b/PKMN_BackUp/PKMN_PokemonHold.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fb155657ce99443/Documents/2017 - ENSAE 2A/S1/Projet C^M^M/rpg-pokemon/PKMN_BackUp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrie\OneDrive\Documents\2017 - ENSAE 2A\S1\Projet C++\rpg-pokemon\PKMN_BackUp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="C52D940A6A74FBFCC37D34A20B5067E25C3BE882" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{D229C94E-5A6A-4188-AC0F-FD59A997FF0E}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="C52D940A6A74FBFCC37D34A20B5067E25C3BE882" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{E558F329-4381-4C95-80F9-356429B4E942}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{AD52951A-4E47-4D22-ACCE-9C73E4EEC872}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>Position</t>
   </si>
@@ -76,6 +76,39 @@
   </si>
   <si>
     <t>20,20,20,20,20,20</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Nidorina</t>
+  </si>
+  <si>
+    <t>128,20,20,20,20,20</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Sandslash</t>
+  </si>
+  <si>
+    <t>Raichu</t>
+  </si>
+  <si>
+    <t>Sandshrew</t>
+  </si>
+  <si>
+    <t>Arbok</t>
+  </si>
+  <si>
+    <t>Fearow</t>
+  </si>
+  <si>
+    <t>255,255,255,255,255,255</t>
   </si>
 </sst>
 </file>
@@ -427,22 +460,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B84C65-31A2-400A-A69F-3CDF88CAE932}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="A1:H7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,178 +484,220 @@
         <v>14</v>
       </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>13</v>
       </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2">
         <v>100</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
       </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3">
         <v>100</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
         <v>15</v>
       </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4">
         <v>100</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
       </c>
       <c r="F4" t="s">
         <v>5</v>
       </c>
       <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
         <v>16</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>15</v>
       </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5">
         <v>100</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
       </c>
       <c r="F5" t="s">
         <v>5</v>
       </c>
       <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>15</v>
       </c>
+      <c r="J5" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6">
         <v>100</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>5</v>
       </c>
       <c r="F6" t="s">
         <v>5</v>
       </c>
       <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
         <v>16</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>15</v>
       </c>
+      <c r="J6" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7">
         <v>100</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
       </c>
       <c r="F7" t="s">
         <v>5</v>
       </c>
       <c r="G7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" t="s">
         <v>16</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>15</v>
+      </c>
+      <c r="J7" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>